<commit_message>
Siege engine bow limit fix
</commit_message>
<xml_diff>
--- a/src/assets/data/mesbg_data.xlsx
+++ b/src/assets/data/mesbg_data.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\alex_\Downloads\mesbg-list-builder-v2024\src\assets\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{95686D0E-FC9C-443C-B817-A52829595D69}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{112A5090-A4AD-4945-91A9-C5CC0E668B9F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="25820" windowHeight="15500" xr2:uid="{41642CF3-1564-4507-B9B3-31F38315AF34}"/>
   </bookViews>
@@ -10234,9 +10234,9 @@
   <sheetPr filterMode="1"/>
   <dimension ref="A1:O738"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="E1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A41" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="N166" sqref="N166"/>
+    <sheetView tabSelected="1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A51" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="L516" sqref="L516"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -12008,7 +12008,7 @@
       </c>
       <c r="O40" s="18"/>
     </row>
-    <row r="41" spans="1:15" x14ac:dyDescent="0.35">
+    <row r="41" spans="1:15" hidden="1" x14ac:dyDescent="0.35">
       <c r="A41" s="18" t="s">
         <v>383</v>
       </c>
@@ -12094,7 +12094,7 @@
       </c>
       <c r="O42" s="18"/>
     </row>
-    <row r="43" spans="1:15" x14ac:dyDescent="0.35">
+    <row r="43" spans="1:15" hidden="1" x14ac:dyDescent="0.35">
       <c r="A43" s="18" t="s">
         <v>390</v>
       </c>
@@ -12442,7 +12442,7 @@
       </c>
       <c r="O50" s="18"/>
     </row>
-    <row r="51" spans="1:15" hidden="1" x14ac:dyDescent="0.35">
+    <row r="51" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A51" s="18" t="s">
         <v>417</v>
       </c>
@@ -12614,7 +12614,7 @@
       </c>
       <c r="O54" s="18"/>
     </row>
-    <row r="55" spans="1:15" x14ac:dyDescent="0.35">
+    <row r="55" spans="1:15" hidden="1" x14ac:dyDescent="0.35">
       <c r="A55" s="18" t="s">
         <v>510</v>
       </c>
@@ -16270,7 +16270,7 @@
       </c>
       <c r="O138" s="18"/>
     </row>
-    <row r="139" spans="1:15" hidden="1" x14ac:dyDescent="0.35">
+    <row r="139" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A139" s="18" t="s">
         <v>760</v>
       </c>
@@ -17310,7 +17310,7 @@
       </c>
       <c r="O162" s="18"/>
     </row>
-    <row r="163" spans="1:15" hidden="1" x14ac:dyDescent="0.35">
+    <row r="163" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A163" s="18" t="s">
         <v>801</v>
       </c>
@@ -17353,7 +17353,7 @@
       </c>
       <c r="O163" s="18"/>
     </row>
-    <row r="164" spans="1:15" x14ac:dyDescent="0.35">
+    <row r="164" spans="1:15" hidden="1" x14ac:dyDescent="0.35">
       <c r="A164" s="18" t="s">
         <v>802</v>
       </c>
@@ -17439,7 +17439,7 @@
       </c>
       <c r="O165" s="18"/>
     </row>
-    <row r="166" spans="1:15" x14ac:dyDescent="0.35">
+    <row r="166" spans="1:15" hidden="1" x14ac:dyDescent="0.35">
       <c r="A166" s="18" t="s">
         <v>804</v>
       </c>
@@ -21136,7 +21136,7 @@
       </c>
       <c r="O250" s="18"/>
     </row>
-    <row r="251" spans="1:15" x14ac:dyDescent="0.35">
+    <row r="251" spans="1:15" hidden="1" x14ac:dyDescent="0.35">
       <c r="A251" s="18" t="s">
         <v>929</v>
       </c>
@@ -21265,7 +21265,7 @@
       </c>
       <c r="O253" s="18"/>
     </row>
-    <row r="254" spans="1:15" x14ac:dyDescent="0.35">
+    <row r="254" spans="1:15" hidden="1" x14ac:dyDescent="0.35">
       <c r="A254" s="18" t="s">
         <v>934</v>
       </c>
@@ -23019,7 +23019,7 @@
       </c>
       <c r="O293" s="18"/>
     </row>
-    <row r="294" spans="1:15" x14ac:dyDescent="0.35">
+    <row r="294" spans="1:15" hidden="1" x14ac:dyDescent="0.35">
       <c r="A294" s="18" t="s">
         <v>1000</v>
       </c>
@@ -23674,7 +23674,7 @@
       </c>
       <c r="O308" s="18"/>
     </row>
-    <row r="309" spans="1:15" x14ac:dyDescent="0.35">
+    <row r="309" spans="1:15" hidden="1" x14ac:dyDescent="0.35">
       <c r="A309" s="18" t="s">
         <v>1026</v>
       </c>
@@ -24415,7 +24415,7 @@
       </c>
       <c r="O325" s="18"/>
     </row>
-    <row r="326" spans="1:15" x14ac:dyDescent="0.35">
+    <row r="326" spans="1:15" hidden="1" x14ac:dyDescent="0.35">
       <c r="A326" s="18" t="s">
         <v>1044</v>
       </c>
@@ -24677,7 +24677,7 @@
       </c>
       <c r="O331" s="18"/>
     </row>
-    <row r="332" spans="1:15" x14ac:dyDescent="0.35">
+    <row r="332" spans="1:15" hidden="1" x14ac:dyDescent="0.35">
       <c r="A332" s="18" t="s">
         <v>1052</v>
       </c>
@@ -25504,7 +25504,7 @@
       </c>
       <c r="O350" s="18"/>
     </row>
-    <row r="351" spans="1:15" x14ac:dyDescent="0.35">
+    <row r="351" spans="1:15" hidden="1" x14ac:dyDescent="0.35">
       <c r="A351" s="18" t="s">
         <v>1077</v>
       </c>
@@ -27039,7 +27039,7 @@
       </c>
       <c r="O385" s="18"/>
     </row>
-    <row r="386" spans="1:15" x14ac:dyDescent="0.35">
+    <row r="386" spans="1:15" hidden="1" x14ac:dyDescent="0.35">
       <c r="A386" s="18" t="s">
         <v>1914</v>
       </c>
@@ -30953,7 +30953,7 @@
         <v>3</v>
       </c>
       <c r="L475" s="18" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="M475" s="18"/>
       <c r="N475" s="18" t="s">
@@ -31866,7 +31866,7 @@
       </c>
       <c r="O496" s="18"/>
     </row>
-    <row r="497" spans="1:15" x14ac:dyDescent="0.35">
+    <row r="497" spans="1:15" hidden="1" x14ac:dyDescent="0.35">
       <c r="A497" s="18" t="s">
         <v>2122</v>
       </c>
@@ -32341,7 +32341,7 @@
       </c>
       <c r="O507" s="18"/>
     </row>
-    <row r="508" spans="1:15" x14ac:dyDescent="0.35">
+    <row r="508" spans="1:15" hidden="1" x14ac:dyDescent="0.35">
       <c r="A508" s="18" t="s">
         <v>2140</v>
       </c>
@@ -32724,7 +32724,7 @@
         <v>1</v>
       </c>
       <c r="L516" s="18" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="M516" s="18"/>
       <c r="N516" s="18" t="s">
@@ -35723,7 +35723,7 @@
       </c>
       <c r="O585" s="18"/>
     </row>
-    <row r="586" spans="1:15" x14ac:dyDescent="0.35">
+    <row r="586" spans="1:15" hidden="1" x14ac:dyDescent="0.35">
       <c r="A586" s="18" t="s">
         <v>2248</v>
       </c>
@@ -40683,21 +40683,9 @@
     </row>
   </sheetData>
   <autoFilter ref="A1:O684" xr:uid="{7E32720F-3682-46D9-B418-543447137BE7}">
-    <filterColumn colId="13">
+    <filterColumn colId="5">
       <filters>
-        <filter val="[['Bain, Son of Bard', '0:1:2:1'], ['Sigrid', '0:1:2:1'], ['Tilda', '0:1:2:1']]"/>
-        <filter val="[['Corsair Ballista - Siege Veteran', '1:1:1:1']]"/>
-        <filter val="[['Eowyn', '2:2:3:2'], ['Meriadoc Brandybuck', '1:1:2:2']]"/>
-        <filter val="[['Gandalf the White', '3:6:3:3']]"/>
-        <filter val="[['Gondor Battlecry Trebuchet - Siege Veteran', '1:1:1:1']]"/>
-        <filter val="[['Haradrim Commander', '2:1:1:2'], ['War Mumak of Harad', '0:0:0:10']]"/>
-        <filter val="[['Iron Hills Ballista - Siege Veteran', '1:1:1:1']]"/>
-        <filter val="[['Isengard Assault Ballista - Siege Veteran', '1:1:1:1']]"/>
-        <filter val="[['Mumak War Leader', '3:2:2:3'], ['Royal War Mumak', '0:0:0:10']]"/>
-        <filter val="[['Shank', '2:3:1:2'], ['Wrot', '1:1:1:2']]"/>
-        <filter val="[['Treebeard', '3:4:3:4']]"/>
-        <filter val="[['Troll Brute', '0:0:0:4'],['Orc Commander', '1:1:1:2']]"/>
-        <filter val="[['Windlance - Siege Veteran', '1:1:1:1']]"/>
+        <filter val="Siege Engine"/>
       </filters>
     </filterColumn>
   </autoFilter>

</xml_diff>

<commit_message>
Arwen - frodo passenger option
</commit_message>
<xml_diff>
--- a/src/assets/data/mesbg_data.xlsx
+++ b/src/assets/data/mesbg_data.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\alex_\Downloads\mesbg-list-builder-v2024\src\assets\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{112A5090-A4AD-4945-91A9-C5CC0E668B9F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{305A544F-94DC-4704-A3A4-27906D18F9DA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="25820" windowHeight="15500" xr2:uid="{41642CF3-1564-4507-B9B3-31F38315AF34}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="25820" windowHeight="15500" activeTab="1" xr2:uid="{41642CF3-1564-4507-B9B3-31F38315AF34}"/>
   </bookViews>
   <sheets>
     <sheet name="models" sheetId="1" r:id="rId1"/>
@@ -49,7 +49,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="10085" uniqueCount="2804">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="10089" uniqueCount="2805">
   <si>
     <t>name</t>
   </si>
@@ -9483,6 +9483,9 @@
   </si>
   <si>
     <t>OPT0873</t>
+  </si>
+  <si>
+    <t>OPT0874</t>
   </si>
 </sst>
 </file>
@@ -10234,9 +10237,9 @@
   <sheetPr filterMode="1"/>
   <dimension ref="A1:O738"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+    <sheetView zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A51" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="L516" sqref="L516"/>
+      <selection pane="bottomLeft" activeCell="A186" sqref="A186"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -12442,7 +12445,7 @@
       </c>
       <c r="O50" s="18"/>
     </row>
-    <row r="51" spans="1:15" x14ac:dyDescent="0.35">
+    <row r="51" spans="1:15" hidden="1" x14ac:dyDescent="0.35">
       <c r="A51" s="18" t="s">
         <v>417</v>
       </c>
@@ -15486,7 +15489,7 @@
       </c>
       <c r="O120" s="18"/>
     </row>
-    <row r="121" spans="1:15" x14ac:dyDescent="0.35">
+    <row r="121" spans="1:15" hidden="1" x14ac:dyDescent="0.35">
       <c r="A121" s="18" t="s">
         <v>729</v>
       </c>
@@ -16270,7 +16273,7 @@
       </c>
       <c r="O138" s="18"/>
     </row>
-    <row r="139" spans="1:15" x14ac:dyDescent="0.35">
+    <row r="139" spans="1:15" hidden="1" x14ac:dyDescent="0.35">
       <c r="A139" s="18" t="s">
         <v>760</v>
       </c>
@@ -17310,7 +17313,7 @@
       </c>
       <c r="O162" s="18"/>
     </row>
-    <row r="163" spans="1:15" x14ac:dyDescent="0.35">
+    <row r="163" spans="1:15" hidden="1" x14ac:dyDescent="0.35">
       <c r="A163" s="18" t="s">
         <v>801</v>
       </c>
@@ -17957,7 +17960,7 @@
       </c>
       <c r="O177" s="18"/>
     </row>
-    <row r="178" spans="1:15" hidden="1" x14ac:dyDescent="0.35">
+    <row r="178" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A178" s="18" t="s">
         <v>820</v>
       </c>
@@ -18000,7 +18003,7 @@
       </c>
       <c r="O178" s="18"/>
     </row>
-    <row r="179" spans="1:15" hidden="1" x14ac:dyDescent="0.35">
+    <row r="179" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A179" s="18" t="s">
         <v>822</v>
       </c>
@@ -18043,7 +18046,7 @@
       </c>
       <c r="O179" s="18"/>
     </row>
-    <row r="180" spans="1:15" hidden="1" x14ac:dyDescent="0.35">
+    <row r="180" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A180" s="18" t="s">
         <v>823</v>
       </c>
@@ -18086,7 +18089,7 @@
       </c>
       <c r="O180" s="18"/>
     </row>
-    <row r="181" spans="1:15" hidden="1" x14ac:dyDescent="0.35">
+    <row r="181" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A181" s="18" t="s">
         <v>824</v>
       </c>
@@ -18129,7 +18132,7 @@
       </c>
       <c r="O181" s="18"/>
     </row>
-    <row r="182" spans="1:15" hidden="1" x14ac:dyDescent="0.35">
+    <row r="182" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A182" s="18" t="s">
         <v>826</v>
       </c>
@@ -18172,7 +18175,7 @@
       </c>
       <c r="O182" s="18"/>
     </row>
-    <row r="183" spans="1:15" hidden="1" x14ac:dyDescent="0.35">
+    <row r="183" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A183" s="18" t="s">
         <v>827</v>
       </c>
@@ -18215,7 +18218,7 @@
       </c>
       <c r="O183" s="18"/>
     </row>
-    <row r="184" spans="1:15" hidden="1" x14ac:dyDescent="0.35">
+    <row r="184" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A184" s="18" t="s">
         <v>828</v>
       </c>
@@ -18258,7 +18261,7 @@
       </c>
       <c r="O184" s="18"/>
     </row>
-    <row r="185" spans="1:15" hidden="1" x14ac:dyDescent="0.35">
+    <row r="185" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A185" s="18" t="s">
         <v>829</v>
       </c>
@@ -18301,7 +18304,7 @@
       </c>
       <c r="O185" s="18"/>
     </row>
-    <row r="186" spans="1:15" hidden="1" x14ac:dyDescent="0.35">
+    <row r="186" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A186" s="18" t="s">
         <v>831</v>
       </c>
@@ -19308,7 +19311,7 @@
       </c>
       <c r="O208" s="18"/>
     </row>
-    <row r="209" spans="1:15" x14ac:dyDescent="0.35">
+    <row r="209" spans="1:15" hidden="1" x14ac:dyDescent="0.35">
       <c r="A209" s="18" t="s">
         <v>864</v>
       </c>
@@ -23326,7 +23329,7 @@
       </c>
       <c r="O300" s="18"/>
     </row>
-    <row r="301" spans="1:15" x14ac:dyDescent="0.35">
+    <row r="301" spans="1:15" hidden="1" x14ac:dyDescent="0.35">
       <c r="A301" s="18" t="s">
         <v>1009</v>
       </c>
@@ -24157,7 +24160,7 @@
       </c>
       <c r="O319" s="18"/>
     </row>
-    <row r="320" spans="1:15" x14ac:dyDescent="0.35">
+    <row r="320" spans="1:15" hidden="1" x14ac:dyDescent="0.35">
       <c r="A320" s="18" t="s">
         <v>1038</v>
       </c>
@@ -26249,7 +26252,7 @@
       </c>
       <c r="O367" s="18"/>
     </row>
-    <row r="368" spans="1:15" x14ac:dyDescent="0.35">
+    <row r="368" spans="1:15" hidden="1" x14ac:dyDescent="0.35">
       <c r="A368" s="18" t="s">
         <v>1746</v>
       </c>
@@ -26646,7 +26649,7 @@
       </c>
       <c r="O376" s="18"/>
     </row>
-    <row r="377" spans="1:15" x14ac:dyDescent="0.35">
+    <row r="377" spans="1:15" hidden="1" x14ac:dyDescent="0.35">
       <c r="A377" s="18" t="s">
         <v>1758</v>
       </c>
@@ -30918,7 +30921,7 @@
       </c>
       <c r="O474" s="18"/>
     </row>
-    <row r="475" spans="1:15" x14ac:dyDescent="0.35">
+    <row r="475" spans="1:15" hidden="1" x14ac:dyDescent="0.35">
       <c r="A475" s="18" t="s">
         <v>2090</v>
       </c>
@@ -32689,7 +32692,7 @@
       </c>
       <c r="O515" s="18"/>
     </row>
-    <row r="516" spans="1:15" x14ac:dyDescent="0.35">
+    <row r="516" spans="1:15" hidden="1" x14ac:dyDescent="0.35">
       <c r="A516" s="18" t="s">
         <v>2153</v>
       </c>
@@ -40683,9 +40686,9 @@
     </row>
   </sheetData>
   <autoFilter ref="A1:O684" xr:uid="{7E32720F-3682-46D9-B418-543447137BE7}">
-    <filterColumn colId="5">
+    <filterColumn colId="2">
       <filters>
-        <filter val="Siege Engine"/>
+        <filter val="Road to Rivendell"/>
       </filters>
     </filterColumn>
   </autoFilter>
@@ -40704,9 +40707,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6BD621D9-338F-4B24-B8C0-543A62D24772}">
   <dimension ref="A1:I1582"/>
   <sheetViews>
-    <sheetView zoomScale="115" zoomScaleNormal="130" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A706" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="C853" sqref="C853"/>
+    <sheetView tabSelected="1" zoomScale="115" zoomScaleNormal="130" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A844" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="F846" sqref="F846"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -55774,11 +55777,21 @@
       </c>
     </row>
     <row r="846" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A846" s="44"/>
-      <c r="B846" s="21"/>
-      <c r="C846" s="21"/>
-      <c r="D846" s="21"/>
-      <c r="E846" s="21"/>
+      <c r="A846" s="15" t="s">
+        <v>2804</v>
+      </c>
+      <c r="B846" s="18" t="s">
+        <v>831</v>
+      </c>
+      <c r="C846" s="21" t="s">
+        <v>580</v>
+      </c>
+      <c r="D846" s="21">
+        <v>55</v>
+      </c>
+      <c r="E846" s="21" t="s">
+        <v>1709</v>
+      </c>
     </row>
     <row r="847" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A847" s="44"/>

</xml_diff>

<commit_message>
Frodo images in Elven Kingdoms
</commit_message>
<xml_diff>
--- a/src/assets/data/mesbg_data.xlsx
+++ b/src/assets/data/mesbg_data.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\alex_\Downloads\mesbg-list-builder-v2024\src\assets\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{305A544F-94DC-4704-A3A4-27906D18F9DA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7D988FDE-AF62-4240-A7B1-658E51326971}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="25820" windowHeight="15500" activeTab="1" xr2:uid="{41642CF3-1564-4507-B9B3-31F38315AF34}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="25820" windowHeight="15500" activeTab="4" xr2:uid="{41642CF3-1564-4507-B9B3-31F38315AF34}"/>
   </bookViews>
   <sheets>
     <sheet name="models" sheetId="1" r:id="rId1"/>
@@ -49,7 +49,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="10089" uniqueCount="2805">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="10089" uniqueCount="2806">
   <si>
     <t>name</t>
   </si>
@@ -9486,6 +9486,9 @@
   </si>
   <si>
     <t>OPT0874</t>
+  </si>
+  <si>
+    <t>['Frodo Baggins']</t>
   </si>
 </sst>
 </file>
@@ -40707,7 +40710,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6BD621D9-338F-4B24-B8C0-543A62D24772}">
   <dimension ref="A1:I1582"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="115" zoomScaleNormal="130" workbookViewId="0">
+    <sheetView zoomScale="115" zoomScaleNormal="130" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A844" activePane="bottomLeft" state="frozen"/>
       <selection pane="bottomLeft" activeCell="F846" sqref="F846"/>
     </sheetView>
@@ -63733,9 +63736,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{59CB009E-54DD-49E7-AF48-1368091BE4E1}">
   <dimension ref="A1:C547"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A11" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="B21" sqref="B21"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A129" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="C140" sqref="C140"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -65271,7 +65274,7 @@
         <v>1719</v>
       </c>
       <c r="C139" s="15" t="s">
-        <v>61</v>
+        <v>2805</v>
       </c>
     </row>
     <row r="140" spans="1:3" x14ac:dyDescent="0.35">

</xml_diff>

<commit_message>
Revert addition of Frodo option to Arwen in Road to Rivendell
</commit_message>
<xml_diff>
--- a/src/assets/data/mesbg_data.xlsx
+++ b/src/assets/data/mesbg_data.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\alex_\Downloads\mesbg-list-builder-v2024\src\assets\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7D988FDE-AF62-4240-A7B1-658E51326971}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{ADB627F1-2142-462B-A344-B4C35E85277F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="25820" windowHeight="15500" activeTab="4" xr2:uid="{41642CF3-1564-4507-B9B3-31F38315AF34}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="25820" windowHeight="15500" activeTab="1" xr2:uid="{41642CF3-1564-4507-B9B3-31F38315AF34}"/>
   </bookViews>
   <sheets>
     <sheet name="models" sheetId="1" r:id="rId1"/>
@@ -49,7 +49,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="10089" uniqueCount="2806">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="10085" uniqueCount="2804">
   <si>
     <t>name</t>
   </si>
@@ -9483,12 +9483,6 @@
   </si>
   <si>
     <t>OPT0873</t>
-  </si>
-  <si>
-    <t>OPT0874</t>
-  </si>
-  <si>
-    <t>['Frodo Baggins']</t>
   </si>
 </sst>
 </file>
@@ -40708,11 +40702,11 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6BD621D9-338F-4B24-B8C0-543A62D24772}">
-  <dimension ref="A1:I1582"/>
+  <dimension ref="A1:I1581"/>
   <sheetViews>
-    <sheetView zoomScale="115" zoomScaleNormal="130" workbookViewId="0">
+    <sheetView tabSelected="1" zoomScale="115" zoomScaleNormal="130" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A844" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="F846" sqref="F846"/>
+      <selection pane="bottomLeft" activeCell="B845" sqref="B845"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -55780,21 +55774,11 @@
       </c>
     </row>
     <row r="846" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A846" s="15" t="s">
-        <v>2804</v>
-      </c>
-      <c r="B846" s="18" t="s">
-        <v>831</v>
-      </c>
-      <c r="C846" s="21" t="s">
-        <v>580</v>
-      </c>
-      <c r="D846" s="21">
-        <v>55</v>
-      </c>
-      <c r="E846" s="21" t="s">
-        <v>1709</v>
-      </c>
+      <c r="A846" s="44"/>
+      <c r="B846" s="21"/>
+      <c r="C846" s="21"/>
+      <c r="D846" s="21"/>
+      <c r="E846" s="21"/>
     </row>
     <row r="847" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A847" s="44"/>
@@ -55868,14 +55852,14 @@
     </row>
     <row r="857" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A857" s="44"/>
-      <c r="B857" s="21"/>
+      <c r="B857" s="44"/>
       <c r="C857" s="21"/>
       <c r="D857" s="21"/>
       <c r="E857" s="21"/>
     </row>
     <row r="858" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A858" s="44"/>
-      <c r="B858" s="44"/>
+      <c r="B858" s="21"/>
       <c r="C858" s="21"/>
       <c r="D858" s="21"/>
       <c r="E858" s="21"/>
@@ -55924,14 +55908,14 @@
     </row>
     <row r="865" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A865" s="44"/>
-      <c r="B865" s="21"/>
+      <c r="B865" s="44"/>
       <c r="C865" s="21"/>
       <c r="D865" s="21"/>
       <c r="E865" s="21"/>
     </row>
     <row r="866" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A866" s="44"/>
-      <c r="B866" s="44"/>
+      <c r="B866" s="21"/>
       <c r="C866" s="21"/>
       <c r="D866" s="21"/>
       <c r="E866" s="21"/>
@@ -55966,14 +55950,14 @@
     </row>
     <row r="871" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A871" s="44"/>
-      <c r="B871" s="21"/>
+      <c r="B871" s="44"/>
       <c r="C871" s="21"/>
       <c r="D871" s="21"/>
       <c r="E871" s="21"/>
     </row>
     <row r="872" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A872" s="44"/>
-      <c r="B872" s="44"/>
+      <c r="B872" s="21"/>
       <c r="C872" s="21"/>
       <c r="D872" s="21"/>
       <c r="E872" s="21"/>
@@ -56099,14 +56083,14 @@
     </row>
     <row r="890" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A890" s="44"/>
-      <c r="B890" s="21"/>
+      <c r="B890" s="44"/>
       <c r="C890" s="21"/>
       <c r="D890" s="21"/>
       <c r="E890" s="21"/>
     </row>
     <row r="891" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A891" s="44"/>
-      <c r="B891" s="44"/>
+      <c r="B891" s="21"/>
       <c r="C891" s="21"/>
       <c r="D891" s="21"/>
       <c r="E891" s="21"/>
@@ -56127,14 +56111,14 @@
     </row>
     <row r="894" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A894" s="44"/>
-      <c r="B894" s="21"/>
+      <c r="B894" s="44"/>
       <c r="C894" s="21"/>
       <c r="D894" s="21"/>
       <c r="E894" s="21"/>
     </row>
     <row r="895" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A895" s="44"/>
-      <c r="B895" s="44"/>
+      <c r="B895" s="21"/>
       <c r="C895" s="21"/>
       <c r="D895" s="21"/>
       <c r="E895" s="21"/>
@@ -56253,14 +56237,14 @@
     </row>
     <row r="912" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A912" s="44"/>
-      <c r="B912" s="21"/>
+      <c r="B912" s="44"/>
       <c r="C912" s="21"/>
       <c r="D912" s="21"/>
       <c r="E912" s="21"/>
     </row>
     <row r="913" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A913" s="44"/>
-      <c r="B913" s="44"/>
+      <c r="B913" s="21"/>
       <c r="C913" s="21"/>
       <c r="D913" s="21"/>
       <c r="E913" s="21"/>
@@ -56281,14 +56265,14 @@
     </row>
     <row r="916" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A916" s="44"/>
-      <c r="B916" s="21"/>
+      <c r="B916" s="44"/>
       <c r="C916" s="21"/>
       <c r="D916" s="21"/>
       <c r="E916" s="21"/>
     </row>
     <row r="917" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A917" s="44"/>
-      <c r="B917" s="44"/>
+      <c r="B917" s="21"/>
       <c r="C917" s="21"/>
       <c r="D917" s="21"/>
       <c r="E917" s="21"/>
@@ -56309,14 +56293,14 @@
     </row>
     <row r="920" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A920" s="44"/>
-      <c r="B920" s="21"/>
+      <c r="B920" s="44"/>
       <c r="C920" s="21"/>
       <c r="D920" s="21"/>
       <c r="E920" s="21"/>
     </row>
     <row r="921" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A921" s="44"/>
-      <c r="B921" s="44"/>
+      <c r="B921" s="21"/>
       <c r="C921" s="21"/>
       <c r="D921" s="21"/>
       <c r="E921" s="21"/>
@@ -56386,14 +56370,14 @@
     </row>
     <row r="931" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A931" s="44"/>
-      <c r="B931" s="21"/>
+      <c r="B931" s="44"/>
       <c r="C931" s="21"/>
       <c r="D931" s="21"/>
       <c r="E931" s="21"/>
     </row>
     <row r="932" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A932" s="44"/>
-      <c r="B932" s="44"/>
+      <c r="B932" s="21"/>
       <c r="C932" s="21"/>
       <c r="D932" s="21"/>
       <c r="E932" s="21"/>
@@ -56428,21 +56412,21 @@
     </row>
     <row r="937" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A937" s="44"/>
-      <c r="B937" s="21"/>
+      <c r="B937" s="44"/>
       <c r="C937" s="21"/>
       <c r="D937" s="21"/>
       <c r="E937" s="21"/>
     </row>
     <row r="938" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A938" s="44"/>
-      <c r="B938" s="44"/>
+      <c r="B938" s="21"/>
       <c r="C938" s="21"/>
       <c r="D938" s="21"/>
       <c r="E938" s="21"/>
     </row>
     <row r="939" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A939" s="44"/>
-      <c r="B939" s="21"/>
+      <c r="B939" s="44"/>
       <c r="C939" s="21"/>
       <c r="D939" s="21"/>
       <c r="E939" s="21"/>
@@ -56456,7 +56440,7 @@
     </row>
     <row r="941" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A941" s="44"/>
-      <c r="B941" s="44"/>
+      <c r="B941" s="21"/>
       <c r="C941" s="21"/>
       <c r="D941" s="21"/>
       <c r="E941" s="21"/>
@@ -56540,14 +56524,14 @@
     </row>
     <row r="953" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A953" s="44"/>
-      <c r="B953" s="21"/>
+      <c r="B953" s="44"/>
       <c r="C953" s="21"/>
       <c r="D953" s="21"/>
       <c r="E953" s="21"/>
     </row>
     <row r="954" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A954" s="44"/>
-      <c r="B954" s="44"/>
+      <c r="B954" s="21"/>
       <c r="C954" s="21"/>
       <c r="D954" s="21"/>
       <c r="E954" s="21"/>
@@ -56617,21 +56601,21 @@
     </row>
     <row r="964" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A964" s="44"/>
-      <c r="B964" s="21"/>
+      <c r="B964" s="44"/>
       <c r="C964" s="21"/>
       <c r="D964" s="21"/>
       <c r="E964" s="21"/>
     </row>
     <row r="965" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A965" s="44"/>
-      <c r="B965" s="44"/>
+      <c r="B965" s="21"/>
       <c r="C965" s="21"/>
       <c r="D965" s="21"/>
       <c r="E965" s="21"/>
     </row>
     <row r="966" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A966" s="44"/>
-      <c r="B966" s="21"/>
+      <c r="B966" s="44"/>
       <c r="C966" s="21"/>
       <c r="D966" s="21"/>
       <c r="E966" s="21"/>
@@ -56645,7 +56629,7 @@
     </row>
     <row r="968" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A968" s="44"/>
-      <c r="B968" s="44"/>
+      <c r="B968" s="21"/>
       <c r="C968" s="21"/>
       <c r="D968" s="21"/>
       <c r="E968" s="21"/>
@@ -56953,14 +56937,14 @@
     </row>
     <row r="1012" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A1012" s="44"/>
-      <c r="B1012" s="21"/>
+      <c r="B1012" s="44"/>
       <c r="C1012" s="21"/>
       <c r="D1012" s="21"/>
       <c r="E1012" s="21"/>
     </row>
     <row r="1013" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A1013" s="44"/>
-      <c r="B1013" s="44"/>
+      <c r="B1013" s="21"/>
       <c r="C1013" s="21"/>
       <c r="D1013" s="21"/>
       <c r="E1013" s="21"/>
@@ -56988,14 +56972,14 @@
     </row>
     <row r="1017" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A1017" s="44"/>
-      <c r="B1017" s="21"/>
+      <c r="B1017" s="44"/>
       <c r="C1017" s="21"/>
       <c r="D1017" s="21"/>
       <c r="E1017" s="21"/>
     </row>
     <row r="1018" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A1018" s="44"/>
-      <c r="B1018" s="44"/>
+      <c r="B1018" s="21"/>
       <c r="C1018" s="21"/>
       <c r="D1018" s="21"/>
       <c r="E1018" s="21"/>
@@ -57023,14 +57007,14 @@
     </row>
     <row r="1022" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A1022" s="44"/>
-      <c r="B1022" s="21"/>
+      <c r="B1022" s="44"/>
       <c r="C1022" s="21"/>
       <c r="D1022" s="21"/>
       <c r="E1022" s="21"/>
     </row>
     <row r="1023" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A1023" s="44"/>
-      <c r="B1023" s="44"/>
+      <c r="B1023" s="21"/>
       <c r="C1023" s="21"/>
       <c r="D1023" s="21"/>
       <c r="E1023" s="21"/>
@@ -57058,14 +57042,14 @@
     </row>
     <row r="1027" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A1027" s="44"/>
-      <c r="B1027" s="21"/>
+      <c r="B1027" s="44"/>
       <c r="C1027" s="21"/>
       <c r="D1027" s="21"/>
       <c r="E1027" s="21"/>
     </row>
     <row r="1028" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A1028" s="44"/>
-      <c r="B1028" s="44"/>
+      <c r="B1028" s="21"/>
       <c r="C1028" s="21"/>
       <c r="D1028" s="21"/>
       <c r="E1028" s="21"/>
@@ -57079,28 +57063,28 @@
     </row>
     <row r="1030" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A1030" s="44"/>
-      <c r="B1030" s="21"/>
+      <c r="B1030" s="44"/>
       <c r="C1030" s="21"/>
       <c r="D1030" s="21"/>
       <c r="E1030" s="21"/>
     </row>
     <row r="1031" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A1031" s="44"/>
-      <c r="B1031" s="44"/>
+      <c r="B1031" s="21"/>
       <c r="C1031" s="21"/>
       <c r="D1031" s="21"/>
       <c r="E1031" s="21"/>
     </row>
     <row r="1032" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A1032" s="44"/>
-      <c r="B1032" s="21"/>
+      <c r="B1032" s="44"/>
       <c r="C1032" s="21"/>
       <c r="D1032" s="21"/>
       <c r="E1032" s="21"/>
     </row>
     <row r="1033" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A1033" s="44"/>
-      <c r="B1033" s="44"/>
+      <c r="B1033" s="21"/>
       <c r="C1033" s="21"/>
       <c r="D1033" s="21"/>
       <c r="E1033" s="21"/>
@@ -57191,14 +57175,14 @@
     </row>
     <row r="1046" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A1046" s="44"/>
-      <c r="B1046" s="21"/>
+      <c r="B1046" s="44"/>
       <c r="C1046" s="21"/>
       <c r="D1046" s="21"/>
       <c r="E1046" s="21"/>
     </row>
     <row r="1047" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A1047" s="44"/>
-      <c r="B1047" s="44"/>
+      <c r="B1047" s="21"/>
       <c r="C1047" s="21"/>
       <c r="D1047" s="21"/>
       <c r="E1047" s="21"/>
@@ -57240,7 +57224,7 @@
     </row>
     <row r="1053" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A1053" s="44"/>
-      <c r="B1053" s="21"/>
+      <c r="B1053" s="44"/>
       <c r="C1053" s="21"/>
       <c r="D1053" s="21"/>
       <c r="E1053" s="21"/>
@@ -57254,7 +57238,7 @@
     </row>
     <row r="1055" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A1055" s="44"/>
-      <c r="B1055" s="44"/>
+      <c r="B1055" s="21"/>
       <c r="C1055" s="21"/>
       <c r="D1055" s="21"/>
       <c r="E1055" s="21"/>
@@ -57562,17 +57546,15 @@
     </row>
     <row r="1099" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A1099" s="44"/>
-      <c r="B1099" s="21"/>
+      <c r="B1099" s="44"/>
       <c r="C1099" s="21"/>
       <c r="D1099" s="21"/>
       <c r="E1099" s="21"/>
     </row>
     <row r="1100" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A1100" s="44"/>
-      <c r="B1100" s="44"/>
       <c r="C1100" s="21"/>
       <c r="D1100" s="21"/>
-      <c r="E1100" s="21"/>
     </row>
     <row r="1101" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A1101" s="44"/>
@@ -57591,20 +57573,21 @@
     </row>
     <row r="1104" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A1104" s="44"/>
+      <c r="B1104" s="44"/>
       <c r="C1104" s="21"/>
       <c r="D1104" s="21"/>
     </row>
     <row r="1105" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A1105" s="44"/>
-      <c r="B1105" s="44"/>
+      <c r="B1105" s="21"/>
       <c r="C1105" s="21"/>
       <c r="D1105" s="21"/>
     </row>
     <row r="1106" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A1106" s="44"/>
-      <c r="B1106" s="21"/>
       <c r="C1106" s="21"/>
       <c r="D1106" s="21"/>
+      <c r="E1106" s="21"/>
     </row>
     <row r="1107" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A1107" s="44"/>
@@ -57616,12 +57599,12 @@
       <c r="A1108" s="44"/>
       <c r="C1108" s="21"/>
       <c r="D1108" s="21"/>
-      <c r="E1108" s="21"/>
     </row>
     <row r="1109" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A1109" s="44"/>
       <c r="C1109" s="21"/>
       <c r="D1109" s="21"/>
+      <c r="E1109" s="21"/>
     </row>
     <row r="1110" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A1110" s="44"/>
@@ -57633,7 +57616,6 @@
       <c r="A1111" s="44"/>
       <c r="C1111" s="21"/>
       <c r="D1111" s="21"/>
-      <c r="E1111" s="21"/>
     </row>
     <row r="1112" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A1112" s="44"/>
@@ -57744,6 +57726,7 @@
       <c r="A1133" s="44"/>
       <c r="C1133" s="21"/>
       <c r="D1133" s="21"/>
+      <c r="E1133" s="21"/>
     </row>
     <row r="1134" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A1134" s="44"/>
@@ -57755,18 +57738,17 @@
       <c r="A1135" s="44"/>
       <c r="C1135" s="21"/>
       <c r="D1135" s="21"/>
-      <c r="E1135" s="21"/>
     </row>
     <row r="1136" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A1136" s="44"/>
       <c r="C1136" s="21"/>
       <c r="D1136" s="21"/>
+      <c r="E1136" s="21"/>
     </row>
     <row r="1137" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A1137" s="44"/>
       <c r="C1137" s="21"/>
       <c r="D1137" s="21"/>
-      <c r="E1137" s="21"/>
     </row>
     <row r="1138" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A1138" s="44"/>
@@ -57777,6 +57759,7 @@
       <c r="A1139" s="44"/>
       <c r="C1139" s="21"/>
       <c r="D1139" s="21"/>
+      <c r="E1139" s="21"/>
     </row>
     <row r="1140" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A1140" s="44"/>
@@ -57794,7 +57777,6 @@
       <c r="A1142" s="44"/>
       <c r="C1142" s="21"/>
       <c r="D1142" s="21"/>
-      <c r="E1142" s="21"/>
     </row>
     <row r="1143" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A1143" s="44"/>
@@ -57843,97 +57825,97 @@
     </row>
     <row r="1152" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A1152" s="44"/>
+      <c r="B1152" s="21"/>
       <c r="C1152" s="21"/>
       <c r="D1152" s="21"/>
-    </row>
-    <row r="1153" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="E1152" s="21"/>
+    </row>
+    <row r="1153" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A1153" s="44"/>
       <c r="B1153" s="21"/>
       <c r="C1153" s="21"/>
       <c r="D1153" s="21"/>
-      <c r="E1153" s="21"/>
-    </row>
-    <row r="1154" spans="1:5" x14ac:dyDescent="0.35">
+    </row>
+    <row r="1154" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A1154" s="44"/>
       <c r="B1154" s="21"/>
       <c r="C1154" s="21"/>
       <c r="D1154" s="21"/>
     </row>
-    <row r="1155" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="1155" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A1155" s="44"/>
       <c r="B1155" s="21"/>
       <c r="C1155" s="21"/>
       <c r="D1155" s="21"/>
     </row>
-    <row r="1156" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="1156" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A1156" s="44"/>
       <c r="B1156" s="21"/>
       <c r="C1156" s="21"/>
       <c r="D1156" s="21"/>
     </row>
-    <row r="1157" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="1157" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A1157" s="44"/>
       <c r="B1157" s="21"/>
       <c r="C1157" s="21"/>
       <c r="D1157" s="21"/>
     </row>
-    <row r="1158" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="1158" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A1158" s="44"/>
       <c r="B1158" s="21"/>
       <c r="C1158" s="21"/>
       <c r="D1158" s="21"/>
     </row>
-    <row r="1159" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="1159" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A1159" s="44"/>
       <c r="B1159" s="21"/>
       <c r="C1159" s="21"/>
       <c r="D1159" s="21"/>
     </row>
-    <row r="1160" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="1160" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A1160" s="44"/>
       <c r="B1160" s="21"/>
       <c r="C1160" s="21"/>
       <c r="D1160" s="21"/>
     </row>
-    <row r="1161" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="1161" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A1161" s="44"/>
       <c r="B1161" s="21"/>
       <c r="C1161" s="21"/>
       <c r="D1161" s="21"/>
     </row>
-    <row r="1162" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="1162" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A1162" s="44"/>
       <c r="B1162" s="21"/>
       <c r="C1162" s="21"/>
       <c r="D1162" s="21"/>
     </row>
-    <row r="1163" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="1163" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A1163" s="44"/>
-      <c r="B1163" s="21"/>
       <c r="C1163" s="21"/>
       <c r="D1163" s="21"/>
     </row>
-    <row r="1164" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="1164" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A1164" s="44"/>
       <c r="C1164" s="21"/>
       <c r="D1164" s="21"/>
     </row>
-    <row r="1165" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="1165" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A1165" s="44"/>
       <c r="C1165" s="21"/>
       <c r="D1165" s="21"/>
     </row>
-    <row r="1166" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="1166" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A1166" s="44"/>
       <c r="C1166" s="21"/>
       <c r="D1166" s="21"/>
     </row>
-    <row r="1167" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="1167" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A1167" s="44"/>
       <c r="C1167" s="21"/>
       <c r="D1167" s="21"/>
     </row>
-    <row r="1168" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="1168" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A1168" s="44"/>
       <c r="C1168" s="21"/>
       <c r="D1168" s="21"/>
@@ -57962,6 +57944,7 @@
       <c r="A1173" s="44"/>
       <c r="C1173" s="21"/>
       <c r="D1173" s="21"/>
+      <c r="E1173" s="21"/>
     </row>
     <row r="1174" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A1174" s="44"/>
@@ -57973,7 +57956,6 @@
       <c r="A1175" s="44"/>
       <c r="C1175" s="21"/>
       <c r="D1175" s="21"/>
-      <c r="E1175" s="21"/>
     </row>
     <row r="1176" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A1176" s="44"/>
@@ -58024,6 +58006,7 @@
       <c r="A1185" s="44"/>
       <c r="C1185" s="21"/>
       <c r="D1185" s="21"/>
+      <c r="E1185" s="21"/>
     </row>
     <row r="1186" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A1186" s="44"/>
@@ -58035,7 +58018,6 @@
       <c r="A1187" s="44"/>
       <c r="C1187" s="21"/>
       <c r="D1187" s="21"/>
-      <c r="E1187" s="21"/>
     </row>
     <row r="1188" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A1188" s="44"/>
@@ -58044,15 +58026,15 @@
     </row>
     <row r="1189" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A1189" s="44"/>
+      <c r="B1189" s="21"/>
       <c r="C1189" s="21"/>
       <c r="D1189" s="21"/>
+      <c r="E1189" s="21"/>
     </row>
     <row r="1190" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A1190" s="44"/>
-      <c r="B1190" s="21"/>
       <c r="C1190" s="21"/>
       <c r="D1190" s="21"/>
-      <c r="E1190" s="21"/>
     </row>
     <row r="1191" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A1191" s="44"/>
@@ -58078,12 +58060,12 @@
       <c r="A1195" s="44"/>
       <c r="C1195" s="21"/>
       <c r="D1195" s="21"/>
+      <c r="E1195" s="21"/>
     </row>
     <row r="1196" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A1196" s="44"/>
       <c r="C1196" s="21"/>
       <c r="D1196" s="21"/>
-      <c r="E1196" s="21"/>
     </row>
     <row r="1197" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A1197" s="44"/>
@@ -58094,12 +58076,12 @@
       <c r="A1198" s="44"/>
       <c r="C1198" s="21"/>
       <c r="D1198" s="21"/>
+      <c r="E1198" s="21"/>
     </row>
     <row r="1199" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A1199" s="44"/>
       <c r="C1199" s="21"/>
       <c r="D1199" s="21"/>
-      <c r="E1199" s="21"/>
     </row>
     <row r="1200" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A1200" s="44"/>
@@ -58130,12 +58112,12 @@
       <c r="A1205" s="44"/>
       <c r="C1205" s="21"/>
       <c r="D1205" s="21"/>
+      <c r="E1205" s="21"/>
     </row>
     <row r="1206" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A1206" s="44"/>
       <c r="C1206" s="21"/>
       <c r="D1206" s="21"/>
-      <c r="E1206" s="21"/>
     </row>
     <row r="1207" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A1207" s="44"/>
@@ -58219,12 +58201,13 @@
     </row>
     <row r="1223" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A1223" s="44"/>
+      <c r="B1223" s="44"/>
       <c r="C1223" s="21"/>
       <c r="D1223" s="21"/>
     </row>
     <row r="1224" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A1224" s="44"/>
-      <c r="B1224" s="44"/>
+      <c r="B1224" s="21"/>
       <c r="C1224" s="21"/>
       <c r="D1224" s="21"/>
     </row>
@@ -58244,12 +58227,11 @@
       <c r="A1227" s="44"/>
       <c r="B1227" s="21"/>
       <c r="C1227" s="21"/>
-      <c r="D1227" s="21"/>
     </row>
     <row r="1228" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A1228" s="44"/>
-      <c r="B1228" s="21"/>
       <c r="C1228" s="21"/>
+      <c r="D1228" s="21"/>
     </row>
     <row r="1229" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A1229" s="44"/>
@@ -58304,11 +58286,11 @@
     <row r="1239" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A1239" s="44"/>
       <c r="C1239" s="21"/>
-      <c r="D1239" s="21"/>
     </row>
     <row r="1240" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A1240" s="44"/>
       <c r="C1240" s="21"/>
+      <c r="D1240" s="21"/>
     </row>
     <row r="1241" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A1241" s="44"/>
@@ -58317,12 +58299,12 @@
     </row>
     <row r="1242" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A1242" s="44"/>
+      <c r="B1242" s="21"/>
       <c r="C1242" s="21"/>
       <c r="D1242" s="21"/>
     </row>
     <row r="1243" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A1243" s="44"/>
-      <c r="B1243" s="21"/>
       <c r="C1243" s="21"/>
       <c r="D1243" s="21"/>
     </row>
@@ -58354,11 +58336,11 @@
     <row r="1249" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A1249" s="44"/>
       <c r="C1249" s="21"/>
-      <c r="D1249" s="21"/>
     </row>
     <row r="1250" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A1250" s="44"/>
       <c r="C1250" s="21"/>
+      <c r="D1250" s="21"/>
     </row>
     <row r="1251" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A1251" s="44"/>
@@ -58368,7 +58350,6 @@
     <row r="1252" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A1252" s="44"/>
       <c r="C1252" s="21"/>
-      <c r="D1252" s="21"/>
     </row>
     <row r="1253" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A1253" s="44"/>
@@ -58405,6 +58386,7 @@
     <row r="1261" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A1261" s="44"/>
       <c r="C1261" s="21"/>
+      <c r="D1261" s="21"/>
     </row>
     <row r="1262" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A1262" s="44"/>
@@ -58419,17 +58401,17 @@
     <row r="1264" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A1264" s="44"/>
       <c r="C1264" s="21"/>
-      <c r="D1264" s="21"/>
     </row>
     <row r="1265" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A1265" s="44"/>
-      <c r="C1265" s="21"/>
     </row>
     <row r="1266" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A1266" s="44"/>
     </row>
     <row r="1267" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A1267" s="44"/>
+      <c r="C1267" s="21"/>
+      <c r="D1267" s="21"/>
     </row>
     <row r="1268" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A1268" s="44"/>
@@ -58439,7 +58421,6 @@
     <row r="1269" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A1269" s="44"/>
       <c r="C1269" s="21"/>
-      <c r="D1269" s="21"/>
     </row>
     <row r="1270" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A1270" s="44"/>
@@ -58456,6 +58437,7 @@
     <row r="1273" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A1273" s="44"/>
       <c r="C1273" s="21"/>
+      <c r="D1273" s="21"/>
     </row>
     <row r="1274" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A1274" s="44"/>
@@ -58470,7 +58452,6 @@
     <row r="1276" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A1276" s="44"/>
       <c r="C1276" s="21"/>
-      <c r="D1276" s="21"/>
     </row>
     <row r="1277" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A1277" s="44"/>
@@ -58479,6 +58460,7 @@
     <row r="1278" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A1278" s="44"/>
       <c r="C1278" s="21"/>
+      <c r="D1278" s="21"/>
     </row>
     <row r="1279" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A1279" s="44"/>
@@ -58502,8 +58484,10 @@
     </row>
     <row r="1283" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A1283" s="44"/>
+      <c r="B1283" s="21"/>
       <c r="C1283" s="21"/>
       <c r="D1283" s="21"/>
+      <c r="E1283" s="21"/>
     </row>
     <row r="1284" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A1284" s="44"/>
@@ -58535,17 +58519,15 @@
     </row>
     <row r="1288" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A1288" s="44"/>
-      <c r="B1288" s="21"/>
+      <c r="B1288" s="44"/>
       <c r="C1288" s="21"/>
       <c r="D1288" s="21"/>
       <c r="E1288" s="21"/>
     </row>
     <row r="1289" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A1289" s="44"/>
-      <c r="B1289" s="44"/>
       <c r="C1289" s="21"/>
       <c r="D1289" s="21"/>
-      <c r="E1289" s="21"/>
     </row>
     <row r="1290" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A1290" s="44"/>
@@ -58611,6 +58593,7 @@
       <c r="A1302" s="44"/>
       <c r="C1302" s="21"/>
       <c r="D1302" s="21"/>
+      <c r="E1302" s="21"/>
     </row>
     <row r="1303" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A1303" s="44"/>
@@ -58622,7 +58605,6 @@
       <c r="A1304" s="44"/>
       <c r="C1304" s="21"/>
       <c r="D1304" s="21"/>
-      <c r="E1304" s="21"/>
     </row>
     <row r="1305" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A1305" s="44"/>
@@ -58671,6 +58653,7 @@
     </row>
     <row r="1314" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A1314" s="44"/>
+      <c r="B1314" s="21"/>
       <c r="C1314" s="21"/>
       <c r="D1314" s="21"/>
     </row>
@@ -58730,7 +58713,6 @@
     </row>
     <row r="1324" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A1324" s="44"/>
-      <c r="B1324" s="21"/>
       <c r="C1324" s="21"/>
       <c r="D1324" s="21"/>
     </row>
@@ -58757,11 +58739,11 @@
     <row r="1329" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A1329" s="44"/>
       <c r="C1329" s="21"/>
-      <c r="D1329" s="21"/>
     </row>
     <row r="1330" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A1330" s="44"/>
       <c r="C1330" s="21"/>
+      <c r="D1330" s="21"/>
     </row>
     <row r="1331" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A1331" s="44"/>
@@ -58776,11 +58758,11 @@
     <row r="1333" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A1333" s="44"/>
       <c r="C1333" s="21"/>
-      <c r="D1333" s="21"/>
     </row>
     <row r="1334" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A1334" s="44"/>
       <c r="C1334" s="21"/>
+      <c r="D1334" s="21"/>
     </row>
     <row r="1335" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A1335" s="44"/>
@@ -58790,7 +58772,6 @@
     <row r="1336" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A1336" s="44"/>
       <c r="C1336" s="21"/>
-      <c r="D1336" s="21"/>
     </row>
     <row r="1337" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A1337" s="44"/>
@@ -58818,7 +58799,10 @@
     </row>
     <row r="1343" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A1343" s="44"/>
+      <c r="B1343" s="21"/>
       <c r="C1343" s="21"/>
+      <c r="D1343" s="21"/>
+      <c r="E1343" s="21"/>
     </row>
     <row r="1344" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A1344" s="44"/>
@@ -58878,14 +58862,14 @@
     </row>
     <row r="1352" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A1352" s="44"/>
-      <c r="B1352" s="21"/>
+      <c r="B1352" s="44"/>
       <c r="C1352" s="21"/>
       <c r="D1352" s="21"/>
       <c r="E1352" s="21"/>
     </row>
     <row r="1353" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A1353" s="44"/>
-      <c r="B1353" s="44"/>
+      <c r="B1353" s="21"/>
       <c r="C1353" s="21"/>
       <c r="D1353" s="21"/>
       <c r="E1353" s="21"/>
@@ -58920,14 +58904,14 @@
     </row>
     <row r="1358" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A1358" s="44"/>
-      <c r="B1358" s="21"/>
+      <c r="B1358" s="44"/>
       <c r="C1358" s="21"/>
       <c r="D1358" s="21"/>
       <c r="E1358" s="21"/>
     </row>
     <row r="1359" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A1359" s="44"/>
-      <c r="B1359" s="44"/>
+      <c r="B1359" s="21"/>
       <c r="C1359" s="21"/>
       <c r="D1359" s="21"/>
       <c r="E1359" s="21"/>
@@ -58955,14 +58939,14 @@
     </row>
     <row r="1363" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A1363" s="44"/>
-      <c r="B1363" s="21"/>
+      <c r="B1363" s="44"/>
       <c r="C1363" s="21"/>
       <c r="D1363" s="21"/>
       <c r="E1363" s="21"/>
     </row>
     <row r="1364" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A1364" s="44"/>
-      <c r="B1364" s="44"/>
+      <c r="B1364" s="21"/>
       <c r="C1364" s="21"/>
       <c r="D1364" s="21"/>
       <c r="E1364" s="21"/>
@@ -59011,14 +58995,14 @@
     </row>
     <row r="1371" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A1371" s="44"/>
-      <c r="B1371" s="21"/>
+      <c r="B1371" s="44"/>
       <c r="C1371" s="21"/>
       <c r="D1371" s="21"/>
       <c r="E1371" s="21"/>
     </row>
     <row r="1372" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A1372" s="44"/>
-      <c r="B1372" s="44"/>
+      <c r="B1372" s="21"/>
       <c r="C1372" s="21"/>
       <c r="D1372" s="21"/>
       <c r="E1372" s="21"/>
@@ -59053,14 +59037,14 @@
     </row>
     <row r="1377" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A1377" s="44"/>
-      <c r="B1377" s="21"/>
+      <c r="B1377" s="44"/>
       <c r="C1377" s="21"/>
       <c r="D1377" s="21"/>
       <c r="E1377" s="21"/>
     </row>
     <row r="1378" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A1378" s="44"/>
-      <c r="B1378" s="44"/>
+      <c r="B1378" s="21"/>
       <c r="C1378" s="21"/>
       <c r="D1378" s="21"/>
       <c r="E1378" s="21"/>
@@ -59088,7 +59072,7 @@
     </row>
     <row r="1382" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A1382" s="44"/>
-      <c r="B1382" s="21"/>
+      <c r="B1382" s="44"/>
       <c r="C1382" s="21"/>
       <c r="D1382" s="21"/>
       <c r="E1382" s="21"/>
@@ -59102,7 +59086,7 @@
     </row>
     <row r="1384" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A1384" s="44"/>
-      <c r="B1384" s="44"/>
+      <c r="B1384" s="21"/>
       <c r="C1384" s="21"/>
       <c r="D1384" s="21"/>
       <c r="E1384" s="21"/>
@@ -59123,7 +59107,7 @@
     </row>
     <row r="1387" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A1387" s="44"/>
-      <c r="B1387" s="21"/>
+      <c r="B1387" s="44"/>
       <c r="C1387" s="21"/>
       <c r="D1387" s="21"/>
       <c r="E1387" s="21"/>
@@ -59137,31 +59121,31 @@
     </row>
     <row r="1389" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A1389" s="44"/>
-      <c r="B1389" s="44"/>
       <c r="C1389" s="21"/>
       <c r="D1389" s="21"/>
-      <c r="E1389" s="21"/>
     </row>
     <row r="1390" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A1390" s="44"/>
+      <c r="B1390" s="21"/>
       <c r="C1390" s="21"/>
       <c r="D1390" s="21"/>
+      <c r="E1390" s="21"/>
     </row>
     <row r="1391" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A1391" s="44"/>
-      <c r="B1391" s="21"/>
       <c r="C1391" s="21"/>
-      <c r="D1391" s="21"/>
-      <c r="E1391" s="21"/>
     </row>
     <row r="1392" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A1392" s="44"/>
       <c r="C1392" s="21"/>
+      <c r="D1392" s="21"/>
     </row>
     <row r="1393" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A1393" s="44"/>
+      <c r="B1393" s="21"/>
       <c r="C1393" s="21"/>
       <c r="D1393" s="21"/>
+      <c r="E1393" s="21"/>
     </row>
     <row r="1394" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A1394" s="44"/>
@@ -59221,7 +59205,7 @@
     </row>
     <row r="1402" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A1402" s="44"/>
-      <c r="B1402" s="21"/>
+      <c r="B1402" s="44"/>
       <c r="C1402" s="21"/>
       <c r="D1402" s="21"/>
       <c r="E1402" s="21"/>
@@ -59382,10 +59366,9 @@
     </row>
     <row r="1425" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A1425" s="44"/>
-      <c r="B1425" s="44"/>
+      <c r="B1425" s="21"/>
       <c r="C1425" s="21"/>
       <c r="D1425" s="21"/>
-      <c r="E1425" s="21"/>
     </row>
     <row r="1426" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A1426" s="44"/>
@@ -59419,7 +59402,6 @@
     </row>
     <row r="1431" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A1431" s="44"/>
-      <c r="B1431" s="21"/>
       <c r="C1431" s="21"/>
       <c r="D1431" s="21"/>
     </row>
@@ -59430,15 +59412,14 @@
     </row>
     <row r="1433" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A1433" s="44"/>
+      <c r="B1433" s="44"/>
       <c r="C1433" s="21"/>
       <c r="D1433" s="21"/>
+      <c r="E1433" s="21"/>
     </row>
     <row r="1434" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A1434" s="44"/>
-      <c r="B1434" s="44"/>
-      <c r="C1434" s="21"/>
-      <c r="D1434" s="21"/>
-      <c r="E1434" s="21"/>
+      <c r="B1434" s="21"/>
     </row>
     <row r="1435" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A1435" s="44"/>
@@ -59447,10 +59428,11 @@
     <row r="1436" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A1436" s="44"/>
       <c r="B1436" s="21"/>
+      <c r="C1436" s="21"/>
+      <c r="D1436" s="21"/>
     </row>
     <row r="1437" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A1437" s="44"/>
-      <c r="B1437" s="21"/>
       <c r="C1437" s="21"/>
       <c r="D1437" s="21"/>
     </row>
@@ -59466,8 +59448,10 @@
     </row>
     <row r="1440" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A1440" s="44"/>
+      <c r="B1440" s="21"/>
       <c r="C1440" s="21"/>
       <c r="D1440" s="21"/>
+      <c r="E1440" s="21"/>
     </row>
     <row r="1441" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A1441" s="44"/>
@@ -59478,10 +59462,8 @@
     </row>
     <row r="1442" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A1442" s="44"/>
-      <c r="B1442" s="21"/>
       <c r="C1442" s="21"/>
       <c r="D1442" s="21"/>
-      <c r="E1442" s="21"/>
     </row>
     <row r="1443" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A1443" s="44"/>
@@ -59496,11 +59478,11 @@
     <row r="1445" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A1445" s="44"/>
       <c r="C1445" s="21"/>
-      <c r="D1445" s="21"/>
     </row>
     <row r="1446" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A1446" s="44"/>
       <c r="C1446" s="21"/>
+      <c r="D1446" s="21"/>
     </row>
     <row r="1447" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A1447" s="44"/>
@@ -59509,8 +59491,10 @@
     </row>
     <row r="1448" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A1448" s="44"/>
+      <c r="B1448" s="21"/>
       <c r="C1448" s="21"/>
       <c r="D1448" s="21"/>
+      <c r="E1448" s="21"/>
     </row>
     <row r="1449" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A1449" s="44"/>
@@ -59528,10 +59512,8 @@
     </row>
     <row r="1451" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A1451" s="44"/>
-      <c r="B1451" s="21"/>
       <c r="C1451" s="21"/>
       <c r="D1451" s="21"/>
-      <c r="E1451" s="21"/>
     </row>
     <row r="1452" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A1452" s="44"/>
@@ -59542,6 +59524,7 @@
       <c r="A1453" s="44"/>
       <c r="C1453" s="21"/>
       <c r="D1453" s="21"/>
+      <c r="E1453" s="21"/>
     </row>
     <row r="1454" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A1454" s="44"/>
@@ -59785,6 +59768,7 @@
     </row>
     <row r="1494" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A1494" s="44"/>
+      <c r="B1494" s="21"/>
       <c r="C1494" s="21"/>
       <c r="D1494" s="21"/>
       <c r="E1494" s="21"/>
@@ -59805,14 +59789,14 @@
     </row>
     <row r="1497" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A1497" s="44"/>
-      <c r="B1497" s="21"/>
+      <c r="B1497" s="44"/>
       <c r="C1497" s="21"/>
       <c r="D1497" s="21"/>
       <c r="E1497" s="21"/>
     </row>
     <row r="1498" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A1498" s="44"/>
-      <c r="B1498" s="44"/>
+      <c r="B1498" s="21"/>
       <c r="C1498" s="21"/>
       <c r="D1498" s="21"/>
       <c r="E1498" s="21"/>
@@ -59840,15 +59824,15 @@
     </row>
     <row r="1502" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A1502" s="44"/>
-      <c r="B1502" s="21"/>
       <c r="C1502" s="21"/>
       <c r="D1502" s="21"/>
-      <c r="E1502" s="21"/>
     </row>
     <row r="1503" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A1503" s="44"/>
+      <c r="B1503" s="21"/>
       <c r="C1503" s="21"/>
       <c r="D1503" s="21"/>
+      <c r="E1503" s="21"/>
     </row>
     <row r="1504" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A1504" s="44"/>
@@ -59901,14 +59885,14 @@
     </row>
     <row r="1511" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A1511" s="44"/>
-      <c r="B1511" s="21"/>
+      <c r="B1511" s="44"/>
       <c r="C1511" s="21"/>
       <c r="D1511" s="21"/>
       <c r="E1511" s="21"/>
     </row>
     <row r="1512" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A1512" s="44"/>
-      <c r="B1512" s="44"/>
+      <c r="B1512" s="21"/>
       <c r="C1512" s="21"/>
       <c r="D1512" s="21"/>
       <c r="E1512" s="21"/>
@@ -59943,14 +59927,14 @@
     </row>
     <row r="1517" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A1517" s="44"/>
-      <c r="B1517" s="21"/>
+      <c r="B1517" s="44"/>
       <c r="C1517" s="21"/>
       <c r="D1517" s="21"/>
       <c r="E1517" s="21"/>
     </row>
     <row r="1518" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A1518" s="44"/>
-      <c r="B1518" s="44"/>
+      <c r="B1518" s="21"/>
       <c r="C1518" s="21"/>
       <c r="D1518" s="21"/>
       <c r="E1518" s="21"/>
@@ -59978,28 +59962,28 @@
     </row>
     <row r="1522" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A1522" s="44"/>
-      <c r="B1522" s="21"/>
+      <c r="B1522" s="44"/>
       <c r="C1522" s="21"/>
       <c r="D1522" s="21"/>
       <c r="E1522" s="21"/>
     </row>
     <row r="1523" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A1523" s="44"/>
-      <c r="B1523" s="44"/>
+      <c r="B1523" s="21"/>
       <c r="C1523" s="21"/>
       <c r="D1523" s="21"/>
       <c r="E1523" s="21"/>
     </row>
     <row r="1524" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A1524" s="44"/>
-      <c r="B1524" s="21"/>
+      <c r="B1524" s="44"/>
       <c r="C1524" s="21"/>
       <c r="D1524" s="21"/>
       <c r="E1524" s="21"/>
     </row>
     <row r="1525" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A1525" s="44"/>
-      <c r="B1525" s="44"/>
+      <c r="B1525" s="21"/>
       <c r="C1525" s="21"/>
       <c r="D1525" s="21"/>
       <c r="E1525" s="21"/>
@@ -60104,19 +60088,17 @@
     </row>
     <row r="1540" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A1540" s="44"/>
-      <c r="B1540" s="21"/>
       <c r="C1540" s="21"/>
       <c r="D1540" s="21"/>
-      <c r="E1540" s="21"/>
     </row>
     <row r="1541" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A1541" s="44"/>
       <c r="C1541" s="21"/>
-      <c r="D1541" s="21"/>
     </row>
     <row r="1542" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A1542" s="44"/>
       <c r="C1542" s="21"/>
+      <c r="D1542" s="21"/>
     </row>
     <row r="1543" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A1543" s="44"/>
@@ -60125,8 +60107,10 @@
     </row>
     <row r="1544" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A1544" s="44"/>
+      <c r="B1544" s="21"/>
       <c r="C1544" s="21"/>
       <c r="D1544" s="21"/>
+      <c r="E1544" s="21"/>
     </row>
     <row r="1545" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A1545" s="44"/>
@@ -60158,14 +60142,14 @@
     </row>
     <row r="1549" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A1549" s="44"/>
-      <c r="B1549" s="21"/>
+      <c r="B1549" s="44"/>
       <c r="C1549" s="21"/>
       <c r="D1549" s="21"/>
       <c r="E1549" s="21"/>
     </row>
     <row r="1550" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A1550" s="44"/>
-      <c r="B1550" s="44"/>
+      <c r="B1550" s="21"/>
       <c r="C1550" s="21"/>
       <c r="D1550" s="21"/>
       <c r="E1550" s="21"/>
@@ -60193,14 +60177,14 @@
     </row>
     <row r="1554" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A1554" s="44"/>
-      <c r="B1554" s="21"/>
+      <c r="B1554" s="44"/>
       <c r="C1554" s="21"/>
       <c r="D1554" s="21"/>
       <c r="E1554" s="21"/>
     </row>
     <row r="1555" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A1555" s="44"/>
-      <c r="B1555" s="44"/>
+      <c r="B1555" s="21"/>
       <c r="C1555" s="21"/>
       <c r="D1555" s="21"/>
       <c r="E1555" s="21"/>
@@ -60277,14 +60261,14 @@
     </row>
     <row r="1566" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A1566" s="44"/>
-      <c r="B1566" s="21"/>
+      <c r="B1566" s="44"/>
       <c r="C1566" s="21"/>
       <c r="D1566" s="21"/>
       <c r="E1566" s="21"/>
     </row>
     <row r="1567" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A1567" s="44"/>
-      <c r="B1567" s="44"/>
+      <c r="B1567" s="21"/>
       <c r="C1567" s="21"/>
       <c r="D1567" s="21"/>
       <c r="E1567" s="21"/>
@@ -60319,14 +60303,14 @@
     </row>
     <row r="1572" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A1572" s="44"/>
-      <c r="B1572" s="21"/>
+      <c r="B1572" s="44"/>
       <c r="C1572" s="21"/>
       <c r="D1572" s="21"/>
       <c r="E1572" s="21"/>
     </row>
     <row r="1573" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A1573" s="44"/>
-      <c r="B1573" s="44"/>
+      <c r="B1573" s="21"/>
       <c r="C1573" s="21"/>
       <c r="D1573" s="21"/>
       <c r="E1573" s="21"/>
@@ -60354,17 +60338,15 @@
     </row>
     <row r="1577" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A1577" s="44"/>
-      <c r="B1577" s="21"/>
+      <c r="B1577" s="44"/>
       <c r="C1577" s="21"/>
       <c r="D1577" s="21"/>
       <c r="E1577" s="21"/>
     </row>
     <row r="1578" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A1578" s="44"/>
-      <c r="B1578" s="44"/>
       <c r="C1578" s="21"/>
       <c r="D1578" s="21"/>
-      <c r="E1578" s="21"/>
     </row>
     <row r="1579" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A1579" s="44"/>
@@ -60378,20 +60360,15 @@
     </row>
     <row r="1581" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A1581" s="44"/>
+      <c r="B1581" s="21"/>
       <c r="C1581" s="21"/>
       <c r="D1581" s="21"/>
-    </row>
-    <row r="1582" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A1582" s="44"/>
-      <c r="B1582" s="21"/>
-      <c r="C1582" s="21"/>
-      <c r="D1582" s="21"/>
-      <c r="E1582" s="21"/>
+      <c r="E1581" s="21"/>
     </row>
   </sheetData>
   <autoFilter ref="A1:I845" xr:uid="{6BD621D9-338F-4B24-B8C0-543A62D24772}"/>
-  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:E1436">
-    <sortCondition ref="A1:A1436"/>
+  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:E1435">
+    <sortCondition ref="A1:A1435"/>
   </sortState>
   <phoneticPr fontId="1" type="noConversion"/>
   <conditionalFormatting sqref="A1:A1048576">
@@ -63736,8 +63713,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{59CB009E-54DD-49E7-AF48-1368091BE4E1}">
   <dimension ref="A1:C547"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A129" activePane="bottomLeft" state="frozen"/>
+    <sheetView workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A132" activePane="bottomLeft" state="frozen"/>
       <selection pane="bottomLeft" activeCell="C140" sqref="C140"/>
     </sheetView>
   </sheetViews>
@@ -65274,7 +65251,7 @@
         <v>1719</v>
       </c>
       <c r="C139" s="15" t="s">
-        <v>2805</v>
+        <v>61</v>
       </c>
     </row>
     <row r="140" spans="1:3" x14ac:dyDescent="0.35">

</xml_diff>